<commit_message>
Atualizações de diagramas e formulários
Criado novo diagrama para gestão da ARP e formulários associados.
</commit_message>
<xml_diff>
--- a/UC1-Pt-br/Tabelas/E-Bidding-0040-2021.xlsx
+++ b/UC1-Pt-br/Tabelas/E-Bidding-0040-2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\DGLC\Projetos\SMART-SC\UC1-gestao-da-lista-basica-de-materiais\Tabelas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\DGLC\Projetos\SMART-SC\UC1-gestao-da-lista-basica-de-materiais\UC1-Pt-br\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E82FEC6-6B2D-4B26-8E47-F7185C0FC046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7A2A0B-AAC8-422A-B52E-301A4E10508C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{39894E0C-A688-4974-9BC1-888E0F07AA26}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39894E0C-A688-4974-9BC1-888E0F07AA26}"/>
   </bookViews>
   <sheets>
     <sheet name="ARP-Campos" sheetId="1" r:id="rId1"/>
@@ -1229,14 +1229,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1722FB1-19BD-4B87-A9A9-C1DC7DBFCF3C}">
   <dimension ref="A1:AA48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.88671875" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
     <col min="6" max="10" width="8.88671875" customWidth="1"/>
@@ -1263,7 +1263,7 @@
       <c r="A1" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -1346,7 +1346,7 @@
       <c r="A2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E2" t="s">
@@ -1390,7 +1390,7 @@
       <c r="A3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E3" t="s">
@@ -1434,7 +1434,7 @@
       <c r="A4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E4" t="s">
@@ -1478,7 +1478,7 @@
       <c r="A5" t="s">
         <v>64</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E5" t="s">
@@ -1522,7 +1522,7 @@
       <c r="A6" t="s">
         <v>64</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E6" t="s">
@@ -1566,7 +1566,7 @@
       <c r="A7" t="s">
         <v>64</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E7" t="s">
@@ -1610,7 +1610,7 @@
       <c r="A8" t="s">
         <v>64</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>68</v>
       </c>
       <c r="E8" t="s">
@@ -1654,7 +1654,7 @@
       <c r="A9" t="s">
         <v>64</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E9" t="s">
@@ -1698,7 +1698,7 @@
       <c r="A10" t="s">
         <v>64</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E10" t="s">
@@ -1742,7 +1742,7 @@
       <c r="A11" t="s">
         <v>64</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E11" t="s">
@@ -1786,7 +1786,7 @@
       <c r="A12" t="s">
         <v>64</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E12" t="s">
@@ -1830,7 +1830,7 @@
       <c r="A13" t="s">
         <v>64</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E13" t="s">
@@ -1874,7 +1874,7 @@
       <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E14" t="s">
@@ -1918,7 +1918,7 @@
       <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E15" t="s">
@@ -1962,7 +1962,7 @@
       <c r="A16" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E16" t="s">
@@ -2006,7 +2006,7 @@
       <c r="A17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E17" t="s">
@@ -2050,7 +2050,7 @@
       <c r="A18" t="s">
         <v>64</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E18" t="s">
@@ -2094,7 +2094,7 @@
       <c r="A19" t="s">
         <v>64</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E19" t="s">
@@ -2138,7 +2138,7 @@
       <c r="A20" t="s">
         <v>64</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E20" t="s">
@@ -2182,7 +2182,7 @@
       <c r="A21" t="s">
         <v>64</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E21" t="s">
@@ -2226,7 +2226,7 @@
       <c r="A22" t="s">
         <v>64</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E22" t="s">
@@ -2270,7 +2270,7 @@
       <c r="A23" t="s">
         <v>64</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E23" t="s">
@@ -2314,7 +2314,7 @@
       <c r="A24" t="s">
         <v>64</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E24" t="s">
@@ -2358,7 +2358,7 @@
       <c r="A25" t="s">
         <v>64</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E25" t="s">
@@ -2402,7 +2402,7 @@
       <c r="A26" t="s">
         <v>64</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E26" t="s">
@@ -2446,7 +2446,7 @@
       <c r="A27" t="s">
         <v>64</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E27" t="s">
@@ -2490,7 +2490,7 @@
       <c r="A28" t="s">
         <v>64</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E28" t="s">
@@ -2534,7 +2534,7 @@
       <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E29" t="s">
@@ -2578,7 +2578,7 @@
       <c r="A30" t="s">
         <v>64</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E30" t="s">
@@ -2622,7 +2622,7 @@
       <c r="A31" t="s">
         <v>64</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E31" t="s">
@@ -2666,7 +2666,7 @@
       <c r="A32" t="s">
         <v>64</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E32" t="s">
@@ -2710,7 +2710,7 @@
       <c r="A33" t="s">
         <v>64</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E33" t="s">
@@ -2754,7 +2754,7 @@
       <c r="A34" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E34" t="s">
@@ -2798,7 +2798,7 @@
       <c r="A35" t="s">
         <v>64</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E35" t="s">
@@ -2842,7 +2842,7 @@
       <c r="A36" t="s">
         <v>64</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E36" t="s">
@@ -2886,7 +2886,7 @@
       <c r="A37" t="s">
         <v>64</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E37" t="s">
@@ -2930,7 +2930,7 @@
       <c r="A38" t="s">
         <v>64</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E38" t="s">
@@ -2974,7 +2974,7 @@
       <c r="A39" t="s">
         <v>64</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E39" t="s">
@@ -3018,7 +3018,7 @@
       <c r="A40" t="s">
         <v>64</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
@@ -3062,7 +3062,7 @@
       <c r="A41" t="s">
         <v>64</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E41" t="s">
@@ -3106,7 +3106,7 @@
       <c r="A42" t="s">
         <v>64</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E42" t="s">
@@ -3150,7 +3150,7 @@
       <c r="A43" t="s">
         <v>64</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E43" t="s">
@@ -3194,7 +3194,7 @@
       <c r="A44" t="s">
         <v>64</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E44" t="s">
@@ -3238,7 +3238,7 @@
       <c r="A45" t="s">
         <v>64</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E45" t="s">
@@ -3282,7 +3282,7 @@
       <c r="A46" t="s">
         <v>64</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E46" t="s">
@@ -3326,7 +3326,7 @@
       <c r="A47" t="s">
         <v>64</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E47" t="s">
@@ -3370,7 +3370,7 @@
       <c r="A48" t="s">
         <v>64</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>75</v>
       </c>
       <c r="E48" t="s">
@@ -3422,7 +3422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC85A58F-E41C-49D5-B72E-F4EB2793BE6C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>